<commit_message>
adjust, title, descr. and delete meta keywords
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\OC\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13705A0E-D4D9-464C-87AB-C683790F5915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E34CCD9-55A0-44E2-9B33-63397C4C4A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="118">
   <si>
     <t>Categorie</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>Mettre le formulaire sur la premiere pages car page n2 contient uniquement le formulaire</t>
+  </si>
+  <si>
+    <t>Fait</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -577,12 +580,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -612,15 +630,6 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -639,6 +648,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -921,103 +949,103 @@
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="28" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1041,158 +1069,158 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="28" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="28" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+    <row r="16" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="34"/>
+      <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
+      <c r="A18" s="32"/>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2199,65 +2227,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E88F27-56C6-4924-8BCC-5C68BFAC9246}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="34.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="122" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="122" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="27"/>
-      <c r="B1" s="36" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="28">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="38" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="28">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="34">
         <v>147</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="34">
         <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="28">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>108</v>
       </c>
       <c r="C4" s="7"/>
@@ -2265,10 +2293,10 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="28">
+      <c r="A5" s="25">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="26" t="s">
         <v>109</v>
       </c>
       <c r="C5" s="7"/>
@@ -2276,51 +2304,61 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="28">
+      <c r="A6" s="25">
         <v>5</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="26" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="28">
+      <c r="A7" s="25">
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="26" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="28">
+      <c r="A8" s="25">
         <v>7</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="26" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="28">
+      <c r="A9" s="25">
         <v>8</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="28">
+      <c r="A10" s="25">
         <v>9</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="26" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="28">
+      <c r="A11" s="25">
         <v>10</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="26" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+    </row>
+    <row r="13" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="41"/>
+      <c r="B13" s="26" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2348,11 +2386,11 @@
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="11" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
delete link in exess (index.html)
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\OC\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8B5A37-A6FE-4B87-ADA9-36439DFC619D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77AEF2-CF2F-4600-A3CA-C8AE67205817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,6 +663,9 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -670,9 +673,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="34.5" x14ac:dyDescent="0.45"/>
@@ -2254,7 +2254,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="42">
+      <c r="A2" s="39">
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -2271,7 +2271,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="42">
+      <c r="A3" s="39">
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -2282,7 +2282,7 @@
       <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="42">
+      <c r="A4" s="39">
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -2293,7 +2293,7 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="42">
+      <c r="A5" s="39">
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
@@ -2304,7 +2304,7 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="25">
+      <c r="A6" s="39">
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -2386,11 +2386,11 @@
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42"/>
       <c r="F1" s="11" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
adjust semantique balise and size and compress img inside html file
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\OC\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77AEF2-CF2F-4600-A3CA-C8AE67205817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FF648C-0D0B-4600-BC2C-74B07F308E40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Mettres des nom de pages addapter</t>
   </si>
   <si>
-    <t xml:space="preserve">avoir des pages nomer en rapport avec le theme et la page actuel au site </t>
-  </si>
-  <si>
     <t>accessibilité</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>Remplacer les images inutiles contenant du texte pars des paragraphe</t>
   </si>
   <si>
-    <t xml:space="preserve">Adapter les taille d'image au conteneur </t>
-  </si>
-  <si>
     <t>Supression des balises li inutiliser</t>
   </si>
   <si>
@@ -373,6 +367,12 @@
   </si>
   <si>
     <t>Remplacer Paris par Lyon</t>
+  </si>
+  <si>
+    <t>Adapter les taille d'image au conteneur et changer les bpm en jpg car se sont des photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir des pages nommer en rapport avec le theme et la page actuel au site </t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,6 +673,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -898,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -969,10 +972,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>53</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -983,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>11</v>
@@ -992,7 +995,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1000,19 +1003,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="D5" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,59 +1023,59 @@
         <v>6</v>
       </c>
       <c r="B6" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="D6" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="E6" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="F6" s="29" t="s">
         <v>37</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>47</v>
-      </c>
       <c r="F7" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="E8" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1080,147 +1083,147 @@
         <v>6</v>
       </c>
       <c r="B9" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="D9" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="E9" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="F9" s="28" t="s">
         <v>99</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="C10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="E10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="F10" s="28" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="D11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>23</v>
-      </c>
       <c r="E11" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="D12" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="E12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>31</v>
-      </c>
       <c r="F12" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="D13" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="E13" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>51</v>
-      </c>
       <c r="F13" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="C14" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="D14" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="E14" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="27" t="s">
-        <v>43</v>
-      </c>
       <c r="F14" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="D15" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="E15" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="F15" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="31"/>
     </row>
@@ -2236,7 +2239,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="34.5" x14ac:dyDescent="0.45"/>
@@ -2250,7 +2253,7 @@
     <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="24"/>
       <c r="B1" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -2258,16 +2261,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="E2" s="35" t="s">
         <v>103</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -2275,7 +2278,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -2286,7 +2289,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -2297,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -2308,23 +2311,23 @@
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="25">
+      <c r="A7" s="43">
         <v>6</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="25">
+      <c r="A8" s="43">
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -2332,23 +2335,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="25">
+      <c r="A10" s="43">
         <v>9</v>
       </c>
       <c r="B10" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="43">
+        <v>10</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="25">
-        <v>10</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2358,7 +2361,7 @@
     <row r="13" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="38"/>
       <c r="B13" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2387,12 +2390,12 @@
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="41"/>
       <c r="E1" s="42"/>
       <c r="F1" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -2417,14 +2420,14 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>59</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -2433,14 +2436,14 @@
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -2449,14 +2452,14 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -2465,14 +2468,14 @@
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
@@ -2481,14 +2484,14 @@
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
@@ -2497,14 +2500,14 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
@@ -2513,14 +2516,14 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
@@ -2529,14 +2532,14 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
@@ -2545,14 +2548,14 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
@@ -2561,14 +2564,14 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>

</xml_diff>

<commit_message>
finsh = reco and adaptation on new seo
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\OC\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FF648C-0D0B-4600-BC2C-74B07F308E40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AC93BC-567B-4A10-993D-8AA1AFFA31F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -666,6 +666,9 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -673,9 +676,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2239,7 +2239,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="34.5" x14ac:dyDescent="0.45"/>
@@ -2315,7 +2315,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="43">
+      <c r="A7" s="40">
         <v>6</v>
       </c>
       <c r="B7" s="26" t="s">
@@ -2323,7 +2323,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="43">
+      <c r="A8" s="40">
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
@@ -2331,7 +2331,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="25">
+      <c r="A9" s="40">
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="43">
+      <c r="A10" s="40">
         <v>9</v>
       </c>
       <c r="B10" s="26" t="s">
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="43">
+      <c r="A11" s="40">
         <v>10</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -2389,11 +2389,11 @@
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="11" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
adjust contrast and accessibility
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\OC\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CAE745-08AF-458C-8FF5-C50B5DCABD2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64035D3-DEB7-41CD-98CA-953115E5C431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>Categorie</t>
   </si>
@@ -182,21 +182,6 @@
     <t>https://cocolyze.com/fr/blog/les-8-regles-seo-pour-optimiser-son-titre-de-page/</t>
   </si>
   <si>
-    <t xml:space="preserve">Certain mots clés ne sont pas vraiment pertinent </t>
-  </si>
-  <si>
-    <t>Faire des recherche avant d'assigner des mots cles</t>
-  </si>
-  <si>
-    <t>Les mots clés comme "design de site web" n'on pas beaucoup de pertinance ! A ne pas confondre avec  "Agence web à paris" qui a le même niveaux de pertinence mais la il sagit d'un mot cles de localisation</t>
-  </si>
-  <si>
-    <t>Faire une recherche de mots clés pour pouvoir remplace les mots cles non-pertinent</t>
-  </si>
-  <si>
-    <t>https://www.seoquantum.com/billet/recherche-mots-cles</t>
-  </si>
-  <si>
     <t>Beaucoup de lien (Non-partenaire)</t>
   </si>
   <si>
@@ -212,9 +197,6 @@
     <t>https://optimiz.me/importance-liens-backlinks-referencement/</t>
   </si>
   <si>
-    <t xml:space="preserve">Page n 2 n'a pas lieu d'ettre </t>
-  </si>
-  <si>
     <t xml:space="preserve">DRY -- Ne pas se répéter </t>
   </si>
   <si>
@@ -288,6 +270,33 @@
   </si>
   <si>
     <t>Répétitions inutile dans le bootstrap.css</t>
+  </si>
+  <si>
+    <t>Methode non apressier de google utiliser</t>
+  </si>
+  <si>
+    <t>Ne pas marquer d'écriture "Invisible" pour le seo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le texte est écrit blanc sur blanc </t>
+  </si>
+  <si>
+    <t>suprimer le texte inutile</t>
+  </si>
+  <si>
+    <t>cour seo</t>
+  </si>
+  <si>
+    <t>le contrast ne rentre pas dans les recommandations google</t>
+  </si>
+  <si>
+    <t>réglé les soucis de contrast</t>
+  </si>
+  <si>
+    <t>la notation du contrast du site est trop faible donc mauvaise pour l'accessibilité du site web</t>
+  </si>
+  <si>
+    <t>faire en sorte d'avoir une notation du contrast corect</t>
   </si>
 </sst>
 </file>
@@ -440,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -505,9 +514,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -740,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="43.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -771,29 +777,29 @@
       <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
+      <c r="A2" s="27"/>
     </row>
     <row r="3" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
@@ -803,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>8</v>
@@ -823,13 +829,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>52</v>
@@ -846,10 +852,10 @@
         <v>22</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>47</v>
@@ -863,10 +869,10 @@
         <v>28</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>29</v>
@@ -880,7 +886,7 @@
         <v>38</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>37</v>
@@ -895,194 +901,201 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>57</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
-        <v>17</v>
-      </c>
       <c r="B11" s="16" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+      <c r="B16" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{BAFF5BC7-B650-46CE-A0E9-4C895F0433B0}"/>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{BAFF5BC7-B650-46CE-A0E9-4C895F0433B0}"/>
     <hyperlink ref="F7" r:id="rId2" xr:uid="{2E8A4EF4-816F-40C3-BCBB-CD0683B3C385}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{D980FE9F-A85B-4132-9BF7-B8F67350C185}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{22C7FC61-D260-4D31-ADF4-38E3717D1562}"/>
-    <hyperlink ref="F12" r:id="rId5" xr:uid="{061504FE-9292-4296-B894-B8BBB5E3372C}"/>
-    <hyperlink ref="F11" r:id="rId6" xr:uid="{F05E7D6F-5CB3-4EF6-8C79-45530220FDA4}"/>
-    <hyperlink ref="F13" r:id="rId7" xr:uid="{FA983050-11FA-4A30-8D5B-5CD63F09F50E}"/>
+    <hyperlink ref="F11" r:id="rId5" xr:uid="{061504FE-9292-4296-B894-B8BBB5E3372C}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{F05E7D6F-5CB3-4EF6-8C79-45530220FDA4}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{FA983050-11FA-4A30-8D5B-5CD63F09F50E}"/>
     <hyperlink ref="F4" r:id="rId8" xr:uid="{115085F0-6E8A-41AE-B652-4205C42BB3FC}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{18BBF607-F7FD-4A2A-9FE4-8332AD2CD0C1}"/>
-    <hyperlink ref="F15" r:id="rId10" xr:uid="{33F9135C-38D4-4740-9DD9-FE912513248C}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{10293114-BD2A-40AA-82A9-449F430F3ABB}"/>
+    <hyperlink ref="F14" r:id="rId9" xr:uid="{33F9135C-38D4-4740-9DD9-FE912513248C}"/>
+    <hyperlink ref="F8" r:id="rId10" xr:uid="{10293114-BD2A-40AA-82A9-449F430F3ABB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId12"/>
+  <pageSetup orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1090,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E88F27-56C6-4924-8BCC-5C68BFAC9246}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1105,7 +1118,7 @@
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1113,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -1124,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1135,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1146,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1157,7 +1170,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1165,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -1173,7 +1186,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -1181,7 +1194,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -1189,7 +1202,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -1197,7 +1210,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -1207,7 +1220,7 @@
     <row r="13" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif semantic balise in HTML
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\OC\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64035D3-DEB7-41CD-98CA-953115E5C431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC3884C-2C0A-4AA5-8597-7F6463C532CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t>Categorie</t>
   </si>
@@ -176,9 +176,6 @@
     <t>http://oseox.fr/referencement/balisage-semantique.html</t>
   </si>
   <si>
-    <t xml:space="preserve">cour html/css . Et un peut de bon sens bon sens </t>
-  </si>
-  <si>
     <t>https://cocolyze.com/fr/blog/les-8-regles-seo-pour-optimiser-son-titre-de-page/</t>
   </si>
   <si>
@@ -296,14 +293,38 @@
     <t>la notation du contrast du site est trop faible donc mauvaise pour l'accessibilité du site web</t>
   </si>
   <si>
-    <t>faire en sorte d'avoir une notation du contrast corect</t>
+    <t xml:space="preserve">beaucoup de balises div </t>
+  </si>
+  <si>
+    <t>utiliser des balises semantique tel que article section etc…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les balises ne sont pas sémantique </t>
+  </si>
+  <si>
+    <t>remplacer les div par des balises semantique</t>
+  </si>
+  <si>
+    <t>https://fr.semrush.com/blog/balises-structurelles-html-semantique/</t>
+  </si>
+  <si>
+    <t>faire en sorte d'avoir une notation du contrast correcte</t>
+  </si>
+  <si>
+    <t>cour html/css . Et un peut de bon sens</t>
+  </si>
+  <si>
+    <t>https://searchengineland.com/how-color-affects-search-engine-optimization-seo-138393</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -368,6 +389,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="8">
@@ -445,9 +471,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -483,51 +510,52 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -746,356 +774,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="43.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="43.33203125" style="23"/>
+    <col min="1" max="1" width="10.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="43.33203125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
+      <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="E5" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="C15" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="C16" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
+      <c r="E17" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1" xr:uid="{BAFF5BC7-B650-46CE-A0E9-4C895F0433B0}"/>
-    <hyperlink ref="F7" r:id="rId2" xr:uid="{2E8A4EF4-816F-40C3-BCBB-CD0683B3C385}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{D980FE9F-A85B-4132-9BF7-B8F67350C185}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{22C7FC61-D260-4D31-ADF4-38E3717D1562}"/>
-    <hyperlink ref="F11" r:id="rId5" xr:uid="{061504FE-9292-4296-B894-B8BBB5E3372C}"/>
-    <hyperlink ref="F10" r:id="rId6" xr:uid="{F05E7D6F-5CB3-4EF6-8C79-45530220FDA4}"/>
-    <hyperlink ref="F12" r:id="rId7" xr:uid="{FA983050-11FA-4A30-8D5B-5CD63F09F50E}"/>
-    <hyperlink ref="F4" r:id="rId8" xr:uid="{115085F0-6E8A-41AE-B652-4205C42BB3FC}"/>
-    <hyperlink ref="F14" r:id="rId9" xr:uid="{33F9135C-38D4-4740-9DD9-FE912513248C}"/>
-    <hyperlink ref="F8" r:id="rId10" xr:uid="{10293114-BD2A-40AA-82A9-449F430F3ABB}"/>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{10293114-BD2A-40AA-82A9-449F430F3ABB}"/>
+    <hyperlink ref="F15" r:id="rId2" xr:uid="{33F9135C-38D4-4740-9DD9-FE912513248C}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{115085F0-6E8A-41AE-B652-4205C42BB3FC}"/>
+    <hyperlink ref="F13" r:id="rId4" xr:uid="{FA983050-11FA-4A30-8D5B-5CD63F09F50E}"/>
+    <hyperlink ref="F11" r:id="rId5" xr:uid="{F05E7D6F-5CB3-4EF6-8C79-45530220FDA4}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{061504FE-9292-4296-B894-B8BBB5E3372C}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{22C7FC61-D260-4D31-ADF4-38E3717D1562}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{D980FE9F-A85B-4132-9BF7-B8F67350C185}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{2E8A4EF4-816F-40C3-BCBB-CD0683B3C385}"/>
+    <hyperlink ref="F10" r:id="rId10" xr:uid="{BAFF5BC7-B650-46CE-A0E9-4C895F0433B0}"/>
+    <hyperlink ref="F8" r:id="rId11" xr:uid="{E02D136F-8D07-4B45-B372-2B5B5CDD7D80}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{104CFEAE-2A7D-4981-98EB-8FF1F52C65CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId11"/>
+  <pageSetup orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1103,7 +1156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E88F27-56C6-4924-8BCC-5C68BFAC9246}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1118,7 +1171,7 @@
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1126,18 +1179,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+        <v>68</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1148,7 +1201,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1159,7 +1212,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1170,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1178,7 +1231,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -1186,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -1194,7 +1247,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -1202,7 +1255,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -1210,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -1220,7 +1273,7 @@
     <row r="13" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minification des fichier css
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pared\Desktop\OC\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC3884C-2C0A-4AA5-8597-7F6463C532CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BEBE94-36B6-4CBC-8FB7-693E53AF29C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="103">
   <si>
     <t>Categorie</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Mettre des lien de partenaria en prioriter, eviter les liens superflux</t>
   </si>
   <si>
-    <t>il y a deux liste de lien qui non seulement prenes de la place et concraitement ne nous servent pas , et se sont des lien au final sans interet pour nôtre site</t>
-  </si>
-  <si>
     <t>Suprimer les liens superflux</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>Methode non apressier de google utiliser</t>
   </si>
   <si>
-    <t>Ne pas marquer d'écriture "Invisible" pour le seo</t>
-  </si>
-  <si>
     <t xml:space="preserve">le texte est écrit blanc sur blanc </t>
   </si>
   <si>
@@ -315,6 +309,114 @@
   </si>
   <si>
     <t>https://searchengineland.com/how-color-affects-search-engine-optimization-seo-138393</t>
+  </si>
+  <si>
+    <t>les documents css et js ne sont pas minifier</t>
+  </si>
+  <si>
+    <t>minifier les fichier a la fin de creation d'un site pour diminuer les temps de chargements</t>
+  </si>
+  <si>
+    <t>les fichiers CSS et JS ne sont pas minifier les temp de chargement en sont impacter</t>
+  </si>
+  <si>
+    <t>minifier les fichier CSS et JS (dans la mesure du possible)</t>
+  </si>
+  <si>
+    <t>http://www.thibautsoufflet.fr/pourquoi-et-comment-minifier-vos-fichiers-css-html-et-javascript/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a deux liste de lien qui non seulement prenes de la place et concraitement ne nous servent pas </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ne pas marquer d'écriture "Invisible" pour le seo (Pratique dite BLACK-HAT qui est puni par</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -324,7 +426,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,8 +497,43 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,8 +576,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -470,13 +613,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -531,26 +842,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="44" fontId="6" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -774,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="43.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -826,329 +1191,350 @@
       <c r="Y1" s="20"/>
       <c r="Z1" s="20"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="36" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="41" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="E8" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="F8" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="E10" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F10" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+    </row>
+    <row r="11" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B11" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C11" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D11" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F11" s="41" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+    <row r="12" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B12" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C12" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D12" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E12" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F12" s="41" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C14" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D14" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E14" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F14" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+    <row r="15" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B15" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C15" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D15" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E15" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="F15" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="E17" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="F17" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="22" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="C18" s="24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="D18" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="22" t="s">
+      <c r="E18" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1" xr:uid="{10293114-BD2A-40AA-82A9-449F430F3ABB}"/>
-    <hyperlink ref="F15" r:id="rId2" xr:uid="{33F9135C-38D4-4740-9DD9-FE912513248C}"/>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{10293114-BD2A-40AA-82A9-449F430F3ABB}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{33F9135C-38D4-4740-9DD9-FE912513248C}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{115085F0-6E8A-41AE-B652-4205C42BB3FC}"/>
-    <hyperlink ref="F13" r:id="rId4" xr:uid="{FA983050-11FA-4A30-8D5B-5CD63F09F50E}"/>
-    <hyperlink ref="F11" r:id="rId5" xr:uid="{F05E7D6F-5CB3-4EF6-8C79-45530220FDA4}"/>
-    <hyperlink ref="F12" r:id="rId6" xr:uid="{061504FE-9292-4296-B894-B8BBB5E3372C}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{FA983050-11FA-4A30-8D5B-5CD63F09F50E}"/>
+    <hyperlink ref="F12" r:id="rId5" xr:uid="{F05E7D6F-5CB3-4EF6-8C79-45530220FDA4}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{061504FE-9292-4296-B894-B8BBB5E3372C}"/>
     <hyperlink ref="F5" r:id="rId7" xr:uid="{22C7FC61-D260-4D31-ADF4-38E3717D1562}"/>
     <hyperlink ref="F3" r:id="rId8" xr:uid="{D980FE9F-A85B-4132-9BF7-B8F67350C185}"/>
     <hyperlink ref="F7" r:id="rId9" xr:uid="{2E8A4EF4-816F-40C3-BCBB-CD0683B3C385}"/>
-    <hyperlink ref="F10" r:id="rId10" xr:uid="{BAFF5BC7-B650-46CE-A0E9-4C895F0433B0}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{BAFF5BC7-B650-46CE-A0E9-4C895F0433B0}"/>
     <hyperlink ref="F8" r:id="rId11" xr:uid="{E02D136F-8D07-4B45-B372-2B5B5CDD7D80}"/>
-    <hyperlink ref="F17" r:id="rId12" xr:uid="{104CFEAE-2A7D-4981-98EB-8FF1F52C65CC}"/>
+    <hyperlink ref="F18" r:id="rId12" xr:uid="{104CFEAE-2A7D-4981-98EB-8FF1F52C65CC}"/>
+    <hyperlink ref="F9" r:id="rId13" xr:uid="{E9EC7E72-6F53-4C4F-A573-EB2E3AEEC773}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId13"/>
+  <pageSetup orientation="landscape" r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -1156,7 +1542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E88F27-56C6-4924-8BCC-5C68BFAC9246}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1171,7 +1557,7 @@
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1179,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1190,7 +1576,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1201,7 +1587,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1212,7 +1598,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1223,7 +1609,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1231,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -1239,7 +1625,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -1247,7 +1633,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -1255,7 +1641,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -1263,7 +1649,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -1273,7 +1659,7 @@
     <row r="13" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>